<commit_message>
Adicionando o .gitignore para remover arquivos de chache e arquivos desnecessarios
</commit_message>
<xml_diff>
--- a/Pasta1.xlsx
+++ b/Pasta1.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
@@ -1414,6 +1414,48 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Renato</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>T.I</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>330</v>
+      </c>
+      <c r="E24" t="n">
+        <v>450</v>
+      </c>
+      <c r="F24" t="n">
+        <v>240</v>
+      </c>
+      <c r="G24" t="n">
+        <v>300</v>
+      </c>
+      <c r="H24" t="n">
+        <v>180</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>22/08/2024</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>